<commit_message>
CF1: Divide adjacent repeat rules. Fix instruments
</commit_message>
<xml_diff>
--- a/MGen/configs/rules/temp.xlsx
+++ b/MGen/configs/rules/temp.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -157,16 +156,16 @@
     <t>sp5</t>
   </si>
   <si>
-    <t>No bass change</t>
-  </si>
-  <si>
-    <t>Bass change</t>
-  </si>
-  <si>
     <t>sp2,3</t>
   </si>
   <si>
     <t>cf/sp1,4</t>
+  </si>
+  <si>
+    <t>No cantus change</t>
+  </si>
+  <si>
+    <t>Cantus change</t>
   </si>
 </sst>
 </file>
@@ -564,31 +563,31 @@
   <dimension ref="A3:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -597,9 +596,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -611,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>

</xml_diff>